<commit_message>
Zeitplan und Umsetzungskonzept aktualisiert am 13.12.2018
</commit_message>
<xml_diff>
--- a/Zeitplanung.xlsx
+++ b/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CH1011687\Desktop\ICT\BLJ\MonitoringPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAA0612-E197-4B24-BC8E-99F8542A81A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B2A0A0-462B-4C03-B5FA-E63B409D9C95}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9744" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="60">
   <si>
     <t>Nr.</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Ist</t>
   </si>
   <si>
-    <t>&lt;Projektname&gt;</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>_</t>
+  </si>
+  <si>
+    <t>MonitoringPro</t>
   </si>
 </sst>
 </file>
@@ -1615,10 +1615,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.25</c:v>
+                  <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2126,7 +2126,7 @@
   <dimension ref="A1:BJ43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2142,7 +2142,7 @@
   <sheetData>
     <row r="1" spans="1:62" ht="25.2" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2247,7 +2247,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="86"/>
       <c r="H3" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -2377,7 +2377,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="22"/>
       <c r="H5" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="6"/>
@@ -2450,13 +2450,13 @@
       </c>
       <c r="D7" s="91"/>
       <c r="E7" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="92" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="92"/>
       <c r="I7" s="92"/>
@@ -2465,7 +2465,7 @@
       <c r="L7" s="92"/>
       <c r="M7" s="93"/>
       <c r="N7" s="92" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O7" s="92"/>
       <c r="P7" s="92"/>
@@ -2474,7 +2474,7 @@
       <c r="S7" s="92"/>
       <c r="T7" s="93"/>
       <c r="U7" s="92" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V7" s="92"/>
       <c r="W7" s="92"/>
@@ -2483,7 +2483,7 @@
       <c r="Z7" s="92"/>
       <c r="AA7" s="93"/>
       <c r="AB7" s="94" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC7" s="92"/>
       <c r="AD7" s="92"/>
@@ -2492,7 +2492,7 @@
       <c r="AG7" s="92"/>
       <c r="AH7" s="93"/>
       <c r="AI7" s="92" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AJ7" s="92"/>
       <c r="AK7" s="92"/>
@@ -2501,7 +2501,7 @@
       <c r="AN7" s="92"/>
       <c r="AO7" s="93"/>
       <c r="AP7" s="94" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AQ7" s="92"/>
       <c r="AR7" s="92"/>
@@ -2510,7 +2510,7 @@
       <c r="AU7" s="92"/>
       <c r="AV7" s="93"/>
       <c r="AW7" s="92" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AX7" s="92"/>
       <c r="AY7" s="92"/>
@@ -2519,7 +2519,7 @@
       <c r="BB7" s="92"/>
       <c r="BC7" s="93"/>
       <c r="BD7" s="94" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="BE7" s="92"/>
       <c r="BF7" s="92"/>
@@ -2543,175 +2543,175 @@
         <v>4</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="L8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="O8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="P8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="R8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="S8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="14" t="s">
+      <c r="T8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="V8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="15" t="s">
+      <c r="W8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="X8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="Z8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="14" t="s">
+      <c r="AD8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="AG8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="S8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="T8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="14" t="s">
+      <c r="AH8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AJ8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="V8" s="15" t="s">
+      <c r="AK8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="W8" s="15" t="s">
+      <c r="AN8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="X8" s="14" t="s">
+      <c r="AR8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AS8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="AT8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Y8" s="14" t="s">
+      <c r="AU8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Z8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB8" s="16" t="s">
+      <c r="AV8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AW8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AC8" s="15" t="s">
+      <c r="AY8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AD8" s="15" t="s">
+      <c r="BB8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="BC8" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="BD8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AE8" s="14" t="s">
+      <c r="BF8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="BG8" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="BH8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AF8" s="14" t="s">
+      <c r="BI8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AG8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AJ8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AK8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AL8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AM8" s="14" t="s">
+      <c r="BJ8" s="25" t="s">
         <v>19</v>
-      </c>
-      <c r="AN8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AO8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AP8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AQ8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AR8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AS8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="AT8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="AU8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AW8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="AX8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="AY8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="AZ8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="BA8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="BB8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="BC8" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="BD8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="BE8" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="BF8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="BG8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="BH8" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="BI8" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="BJ8" s="25" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2719,7 +2719,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="41">
         <f>SUM(C10:C13)</f>
@@ -2796,14 +2796,14 @@
         <v>12</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="84"/>
       <c r="E10" s="48">
         <v>1</v>
       </c>
       <c r="F10" s="88" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="54"/>
@@ -2869,7 +2869,7 @@
         <v>102</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="49">
         <v>3</v>
@@ -2952,7 +2952,7 @@
         <v>103</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="49">
         <v>5</v>
@@ -3029,17 +3029,17 @@
         <v>104</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="50">
         <v>1</v>
       </c>
       <c r="F13" s="88" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="59"/>
       <c r="H13" s="60"/>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>14.25</v>
+        <v>16.25</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3177,7 +3177,7 @@
         <v>201</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="49">
         <v>3</v>
@@ -3190,7 +3190,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="89" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
@@ -3260,14 +3260,14 @@
         <v>202</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="49">
         <v>10</v>
       </c>
       <c r="D16" s="83">
         <f>SUM(G16:BJ16)</f>
-        <v>7.25</v>
+        <v>9.25</v>
       </c>
       <c r="E16" s="50">
         <v>1</v>
@@ -3286,10 +3286,12 @@
       <c r="M16" s="58"/>
       <c r="N16" s="59"/>
       <c r="O16" s="60"/>
-      <c r="P16" s="63" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q16" s="87"/>
+      <c r="P16" s="63">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="87">
+        <v>1</v>
+      </c>
       <c r="R16" s="55"/>
       <c r="S16" s="57"/>
       <c r="T16" s="58"/>
@@ -3418,7 +3420,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3484,14 +3486,14 @@
         <v>301</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="49">
         <v>2</v>
       </c>
       <c r="D19" s="83">
         <f>SUM(G19:BJ19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="50">
         <v>1</v>
@@ -3506,8 +3508,8 @@
       <c r="M19" s="58"/>
       <c r="N19" s="53"/>
       <c r="O19" s="54"/>
-      <c r="P19" s="63" t="s">
-        <v>5</v>
+      <c r="P19" s="63">
+        <v>1</v>
       </c>
       <c r="Q19" s="63" t="s">
         <v>5</v>
@@ -3563,14 +3565,14 @@
         <v>302</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="49">
         <v>10</v>
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E20" s="50">
         <v>1</v>
@@ -3585,8 +3587,8 @@
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
       <c r="O20" s="60"/>
-      <c r="P20" s="63" t="s">
-        <v>5</v>
+      <c r="P20" s="63">
+        <v>6</v>
       </c>
       <c r="Q20" s="63" t="s">
         <v>5</v>
@@ -3642,7 +3644,7 @@
         <v>303</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" s="49">
         <v>2</v>
@@ -3719,7 +3721,7 @@
         <v>304</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C22" s="49">
         <v>2</v>
@@ -3798,7 +3800,7 @@
         <v>305</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" s="49">
         <v>2</v>
@@ -3877,7 +3879,7 @@
         <v>306</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="49">
         <v>2</v>
@@ -3890,7 +3892,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G24" s="59"/>
       <c r="H24" s="60"/>
@@ -3958,7 +3960,7 @@
         <v>307</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="49">
         <v>8</v>
@@ -4035,7 +4037,7 @@
         <v>308</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C26" s="49">
         <v>2</v>
@@ -4110,7 +4112,7 @@
         <v>309</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C27" s="49">
         <v>2</v>
@@ -4466,7 +4468,7 @@
         <v>401</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="49">
         <v>1</v>
@@ -4541,7 +4543,7 @@
         <v>402</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" s="49">
         <v>2</v>
@@ -4616,7 +4618,7 @@
         <v>403</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="49">
         <v>4</v>
@@ -4834,7 +4836,7 @@
         <v>501</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="49">
         <v>5</v>
@@ -5052,7 +5054,7 @@
         <v>601</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="49">
         <v>1</v>
@@ -5127,7 +5129,7 @@
         <v>602</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41" s="49">
         <v>2</v>
@@ -5277,7 +5279,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>18.25</v>
+        <v>27.25</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5319,11 +5321,11 @@
       </c>
       <c r="P43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
@@ -5507,7 +5509,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" scenarios="1" formatCells="0"/>
+  <sheetProtection formatCells="0"/>
   <mergeCells count="9">
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="G7:M7"/>
@@ -5592,7 +5594,7 @@
       </c>
       <c r="D4" s="80">
         <f>Zeitplanung!D14</f>
-        <v>14.25</v>
+        <v>16.25</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
@@ -5609,7 +5611,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>